<commit_message>
Correct the points raised in the first review
</commit_message>
<xml_diff>
--- a/documents/plan/プロジェクト計画書_レビュー記録.xlsx
+++ b/documents/plan/プロジェクト計画書_レビュー記録.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/273debb854664e28/デスクトップ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/273debb854664e28/デスクトップ/Projects/10031s0001/documents/plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{4D580200-F178-42B7-A906-3EE4D5415D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8328B1E7-7A33-4A60-85A5-3EB346D715A1}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{4D580200-F178-42B7-A906-3EE4D5415D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A65F7E31-357A-4021-9104-12B5CAA0B825}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-2205" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{2EC08767-6C6C-4952-9411-FFBC95C883F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EC08767-6C6C-4952-9411-FFBC95C883F7}"/>
   </bookViews>
   <sheets>
     <sheet name="改訂履歴" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2"/>
@@ -174,6 +174,88 @@
     </rPh>
     <rPh sb="2" eb="4">
       <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2.0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>第1回レビューの指摘内容と修正内容を記載</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シテキ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>シュウセイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>キサイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1.はじめに</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4.4 開発検証</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>"4.4 開発検証" にレビュー仕様書とありますが、指摘の管理だと思いますので、"レビュー記録"もしくは"レビュー指摘表"がよいと思います。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>セック光内</t>
+    <rPh sb="3" eb="5">
+      <t>ミツウチ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>"レビュー記録"にファイル名を修正しました。</t>
+    <rPh sb="5" eb="7">
+      <t>キロク</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>PHR舩橋</t>
+    <rPh sb="3" eb="5">
+      <t>フナバシ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>"1.はじめに"の本文最後に意図が不明な"→"が見えます。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>"1.はじめに"の本文最後の不要な"→"を削除しました。</t>
+    <rPh sb="14" eb="16">
+      <t>フヨウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>サクジョ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -185,7 +267,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +293,20 @@
       <color theme="0"/>
       <name val="Meiryo UI"/>
       <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -264,12 +360,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -330,8 +429,21 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -671,10 +783,10 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="13"/>
     <col min="2" max="2" width="13.88671875" style="19" bestFit="1" customWidth="1"/>
@@ -682,7 +794,7 @@
     <col min="4" max="4" width="44.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -696,7 +808,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
@@ -710,55 +822,63 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
+      <c r="A3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="18">
+        <v>45467</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="12"/>
       <c r="B4" s="18"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="12"/>
       <c r="B5" s="18"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="12"/>
       <c r="B6" s="18"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="12"/>
       <c r="B7" s="18"/>
       <c r="C7" s="3"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="12"/>
       <c r="B8" s="18"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="12"/>
       <c r="B9" s="18"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="12"/>
       <c r="B10" s="18"/>
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="12"/>
       <c r="B11" s="18"/>
       <c r="C11" s="3"/>
@@ -775,30 +895,30 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="40.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="23" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="4" customWidth="1"/>
     <col min="6" max="6" width="40.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="12.77734375" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -820,653 +940,677 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="8">
+        <v>45467</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H2" s="8"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="47.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="B3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8">
+        <v>45467</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H3" s="8"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="8"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="1"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="8"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="8"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="8"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="8"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="8"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="1"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="8"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="8"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="8"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="12"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="8"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="8"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="8"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="8"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="12"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="8"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="8"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="12"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="8"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="12"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="8"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="8"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="12"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="8"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="12"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="8"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="3"/>
       <c r="H28" s="8"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="12"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="1"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="8"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="1"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="8"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="12"/>
-      <c r="C31" s="1"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="1"/>
+      <c r="E31" s="3"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="G31" s="3"/>
       <c r="H31" s="8"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="12"/>
-      <c r="C32" s="1"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="8"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="12"/>
-      <c r="C33" s="1"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="1"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="8"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="12"/>
-      <c r="C34" s="1"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="1"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="G34" s="3"/>
       <c r="H34" s="8"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="12"/>
-      <c r="C35" s="1"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="1"/>
+      <c r="E35" s="3"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="G35" s="3"/>
       <c r="H35" s="8"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="12"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="1"/>
+      <c r="E36" s="3"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="G36" s="3"/>
       <c r="H36" s="8"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="12"/>
-      <c r="C37" s="1"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="1"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="G37" s="3"/>
       <c r="H37" s="8"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="12"/>
-      <c r="C38" s="1"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="1"/>
+      <c r="E38" s="3"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="G38" s="3"/>
       <c r="H38" s="8"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="12"/>
-      <c r="C39" s="1"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="1"/>
+      <c r="E39" s="3"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="G39" s="3"/>
       <c r="H39" s="8"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="12"/>
-      <c r="C40" s="1"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="1"/>
+      <c r="E40" s="3"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="G40" s="3"/>
       <c r="H40" s="8"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="12"/>
-      <c r="C41" s="1"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="8"/>
-      <c r="E41" s="1"/>
+      <c r="E41" s="3"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="G41" s="3"/>
       <c r="H41" s="8"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="12"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="22"/>
       <c r="D42" s="8"/>
-      <c r="E42" s="1"/>
+      <c r="E42" s="3"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="G42" s="3"/>
       <c r="H42" s="8"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="12"/>
-      <c r="C43" s="1"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="1"/>
+      <c r="E43" s="3"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="G43" s="3"/>
       <c r="H43" s="8"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="12"/>
-      <c r="C44" s="1"/>
+      <c r="C44" s="22"/>
       <c r="D44" s="8"/>
-      <c r="E44" s="1"/>
+      <c r="E44" s="3"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="G44" s="3"/>
       <c r="H44" s="8"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" s="12"/>
-      <c r="C45" s="1"/>
+      <c r="C45" s="22"/>
       <c r="D45" s="8"/>
-      <c r="E45" s="1"/>
+      <c r="E45" s="3"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="G45" s="3"/>
       <c r="H45" s="8"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="12"/>
-      <c r="C46" s="1"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="8"/>
-      <c r="E46" s="1"/>
+      <c r="E46" s="3"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="G46" s="3"/>
       <c r="H46" s="8"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" s="12"/>
-      <c r="C47" s="1"/>
+      <c r="C47" s="22"/>
       <c r="D47" s="8"/>
-      <c r="E47" s="1"/>
+      <c r="E47" s="3"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="G47" s="3"/>
       <c r="H47" s="8"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="12"/>
-      <c r="C48" s="1"/>
+      <c r="C48" s="22"/>
       <c r="D48" s="8"/>
-      <c r="E48" s="1"/>
+      <c r="E48" s="3"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
+      <c r="G48" s="3"/>
       <c r="H48" s="8"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" s="12"/>
-      <c r="C49" s="1"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="8"/>
-      <c r="E49" s="1"/>
+      <c r="E49" s="3"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="G49" s="3"/>
       <c r="H49" s="8"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="12"/>
-      <c r="C50" s="1"/>
+      <c r="C50" s="22"/>
       <c r="D50" s="8"/>
-      <c r="E50" s="1"/>
+      <c r="E50" s="3"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="G50" s="3"/>
       <c r="H50" s="8"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" s="12"/>
-      <c r="C51" s="1"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="8"/>
-      <c r="E51" s="1"/>
+      <c r="E51" s="3"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="G51" s="3"/>
       <c r="H51" s="8"/>
       <c r="I51" s="1"/>
     </row>

</xml_diff>

<commit_message>
Correct the typographical errors
</commit_message>
<xml_diff>
--- a/documents/plan/プロジェクト計画書_レビュー記録.xlsx
+++ b/documents/plan/プロジェクト計画書_レビュー記録.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/273debb854664e28/デスクトップ/Projects/10031s0001/documents/plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{4D580200-F178-42B7-A906-3EE4D5415D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A65F7E31-357A-4021-9104-12B5CAA0B825}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="8_{4D580200-F178-42B7-A906-3EE4D5415D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E9F2F11-E0F2-4772-A1CE-D26D7C5A515B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EC08767-6C6C-4952-9411-FFBC95C883F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EC08767-6C6C-4952-9411-FFBC95C883F7}"/>
   </bookViews>
   <sheets>
     <sheet name="改訂履歴" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2"/>
@@ -182,31 +182,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>第1回レビューの指摘内容と修正内容を記載</t>
-    <rPh sb="0" eb="1">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シテキ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>シュウセイ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>キサイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>1.はじめに</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -256,6 +231,82 @@
     </rPh>
     <rPh sb="21" eb="23">
       <t>サクジョ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&gt;"4.4 開発検証" にレビュー仕様書とありますが、指摘の管理だと思いますので、"レビュー記録"もしくは"レビュー指摘表"がよいと思います。
+上記本文中に残っています。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4.4開発検証の誤記を修正しました。
+レビュー仕様書 → レビュー記録</t>
+    <rPh sb="3" eb="5">
+      <t>カイハツ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ゴキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>シュウセイ</t>
+    </rPh>
+    <rPh sb="23" eb="26">
+      <t>シヨウショ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>キロク</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2.1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>第1回レビューの指摘内容(No.1~2)と修正内容を記載</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シテキ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>シュウセイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>キサイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No.3の指摘内容と修正内容を記載</t>
+    <rPh sb="5" eb="7">
+      <t>シテキ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>シュウセイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>キサイ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -782,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB19FF1-8D7D-45C7-BC07-A4CD6283F034}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -833,14 +884,22 @@
         <v>14</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="12"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="18">
+        <v>45468</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="12"/>
@@ -894,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25D357B-7C90-4BB4-B54E-4646094FE803}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -945,22 +1004,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="8">
         <v>45467</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="1"/>
@@ -970,36 +1029,48 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>20</v>
       </c>
       <c r="D3" s="8">
         <v>45467</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="63">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="8">
+        <v>45468</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="8"/>
       <c r="I4" s="1"/>
     </row>

</xml_diff>